<commit_message>
Restore front page elements
</commit_message>
<xml_diff>
--- a/support/glossary.xlsx
+++ b/support/glossary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tracyreith/Desktop/Redux-Kitchen/support/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C038947F-0128-DB4E-9C68-C4503A6ED8D7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{198FD60D-A128-7844-8080-A11092F67619}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2980" yWindow="640" windowWidth="13680" windowHeight="16420" xr2:uid="{B945C795-EDD6-5D4E-9417-32859E378990}"/>
+    <workbookView xWindow="10440" yWindow="460" windowWidth="23820" windowHeight="16140" xr2:uid="{B945C795-EDD6-5D4E-9417-32859E378990}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -465,10 +465,13 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="98.1640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">

</xml_diff>